<commit_message>
Replacing Test Case Sample.xlsx
</commit_message>
<xml_diff>
--- a/modules/M15/assets/TestCaseSample.xlsx
+++ b/modules/M15/assets/TestCaseSample.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JosephFord\git\prime-therapeutics-training\modules\M15\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3123A2-89F6-4137-8CE0-C62FFDAC471D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CCCEA9F-2757-4388-A4A4-BD5D3E2A9DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1F7AA7D8-DC19-40D2-BBCC-539A6696B0E6}"/>
+    <workbookView xWindow="4410" yWindow="1935" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{1F7AA7D8-DC19-40D2-BBCC-539A6696B0E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="3" r:id="rId1"/>
-    <sheet name="TC01" sheetId="1" r:id="rId2"/>
-    <sheet name="TC02" sheetId="2" r:id="rId3"/>
+    <sheet name="TC01" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="58">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -69,9 +68,6 @@
     <t>Step 8</t>
   </si>
   <si>
-    <t>Step 9</t>
-  </si>
-  <si>
     <t>Step</t>
   </si>
   <si>
@@ -93,9 +89,6 @@
     <t>TC01</t>
   </si>
   <si>
-    <t>Cancel Adding Valid Field Agent</t>
-  </si>
-  <si>
     <t>Navigate to http://localhost:3000/</t>
   </si>
   <si>
@@ -120,9 +113,6 @@
     <t>Enter "01/01/2001" for Date of Birth</t>
   </si>
   <si>
-    <t>Click Cancel button</t>
-  </si>
-  <si>
     <t>Field Agents main UI displays</t>
   </si>
   <si>
@@ -135,12 +125,6 @@
     <t>Add Valid Field Agent</t>
   </si>
   <si>
-    <t>Field Agents main UI displays. Testy M McTester is not displayed.</t>
-  </si>
-  <si>
-    <t>Add Agent UI displays with empty fields. Previously entered values are lost.</t>
-  </si>
-  <si>
     <t>Field Agents main UI displays. Testy M McTester is displayed.</t>
   </si>
   <si>
@@ -195,9 +179,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>TC02</t>
-  </si>
-  <si>
     <t>M1</t>
   </si>
   <si>
@@ -229,58 +210,13 @@
   </si>
   <si>
     <t>D1</t>
-  </si>
-  <si>
-    <t>Requests for Clarification</t>
-  </si>
-  <si>
-    <t>What if there are 10,000 agents? Should it paginate?</t>
-  </si>
-  <si>
-    <t>Answer</t>
-  </si>
-  <si>
-    <t>Yes, options for 10,50,100, by default 10.</t>
-  </si>
-  <si>
-    <t>What if there are 0 agents? Should it display something indicating there are 0 agents?</t>
-  </si>
-  <si>
-    <t>What should the next sort option be if last name, first name and birthday combination is duplicated?</t>
-  </si>
-  <si>
-    <t>A1,A2,A3</t>
-  </si>
-  <si>
-    <t>Min/max length requirements?</t>
-  </si>
-  <si>
-    <t>Min: 1 character, Max: 255 characters</t>
-  </si>
-  <si>
-    <t>Character Encoding?</t>
-  </si>
-  <si>
-    <t>UTF-8</t>
-  </si>
-  <si>
-    <t>Maximum Age?</t>
-  </si>
-  <si>
-    <t>&lt;Not answered yet&gt;</t>
-  </si>
-  <si>
-    <t>Are partial inches allowed? Expressed as a decimal or fraction?</t>
-  </si>
-  <si>
-    <t>Partial inches are not allowed.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -292,12 +228,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -392,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -400,8 +330,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -733,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{098930DE-8D8D-45DA-A241-A25919227673}">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,293 +674,183 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="11" t="s">
-        <v>49</v>
+      <c r="B1" s="9" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>50</v>
+      <c r="B3" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="11" t="s">
-        <v>40</v>
+      <c r="B9" s="9" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
         <v>46</v>
       </c>
-      <c r="C15" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="11" t="s">
-        <v>47</v>
+      <c r="B17" s="9" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
-      </c>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="10"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="10"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>66</v>
-      </c>
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>76</v>
-      </c>
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="12"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="12"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="12"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="12"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="12"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="12"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="12"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1041,205 +859,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E46303A3-81DA-4707-ABB8-77138E60A104}">
-  <dimension ref="A1:E13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA3EDD90-99AC-4D89-91FF-934F02A79C73}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1251,52 +874,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>52</v>
+      <c r="B1" s="6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>31</v>
+      <c r="B2" s="7" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="E4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="7" t="s">
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="2" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -1304,14 +927,14 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1319,14 +942,14 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1334,14 +957,14 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1349,14 +972,14 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1364,14 +987,14 @@
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1379,14 +1002,14 @@
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1394,14 +1017,14 @@
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>